<commit_message>
Evaluation and join of data-tables from SDTM and MAPPER data (not WWARNset)
</commit_message>
<xml_diff>
--- a/outcomes/pubmed_id.xlsx
+++ b/outcomes/pubmed_id.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juansebastianhurtadozapata/Desktop/CIDEIM/Clinic unit : UBE/TDR application /Fellowship stay IDDO/Malaria Project - Fellow/hyperparasitimia_malaria_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juansebastianhurtadozapata/Desktop/CIDEIM/Clinic unit : UBE/TDR application /Fellowship stay IDDO/Malaria Project - Fellow/hyperparasitimia_malaria_project/outcomes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDA0FE-0F80-474D-9159-DFED362279B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345A7A4-523B-1C49-A719-DC9EDA6AA6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:G17"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>